<commit_message>
Correción de busqueda automatica de nombres
</commit_message>
<xml_diff>
--- a/NFL Quinela 2025.xlsx
+++ b/NFL Quinela 2025.xlsx
@@ -19,6 +19,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="10" sheetId="11" state="visible" r:id="rId11"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11" sheetId="12" state="visible" r:id="rId12"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="12" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="13" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -11643,6 +11644,655 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Judith Fernández Franco</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Green Bay - Packers</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Kansas City - Chiefs</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Baltimore - Ravens (Local)</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Philadelphia - Eagles (Local)</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>San Francisco - 49ers</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Jacksonville - Jaguars</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Indianapolis - Colts (Local)</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Miami - Dolphins (Local)</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Atlanta - Falcons</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Tampa Bay - Buccaneers (Local)</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Los Angeles - Rams</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Seattle - Seahawks (Local)</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Buffalo - Bills</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Los Angeles - Chargers (Local)</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Denver - Broncos</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>New England - Patriots (Local)</t>
+        </is>
+      </c>
+      <c r="R1" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Guiorguio Guitto Sánchez Muñoz</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Detroit - Lions (Local)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Dallas - Cowboys (Local)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Cincinnati - Bengals</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Philadelphia - Eagles (Local)</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>San Francisco - 49ers</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Jacksonville - Jaguars</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Indianapolis - Colts (Local)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Miami - Dolphins (Local)</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>New York - Jets (Local)</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Tampa Bay - Buccaneers (Local)</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Los Angeles - Rams</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Seattle - Seahawks (Local)</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Pittsburgh - Steelers (Local)</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Los Angeles - Chargers (Local)</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Denver - Broncos</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>New England - Patriots (Local)</t>
+        </is>
+      </c>
+      <c r="R2" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Neima Dorely Meza Jáquez</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Green Bay - Packers</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Kansas City - Chiefs</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Baltimore - Ravens (Local)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Philadelphia - Eagles (Local)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Cleveland - Browns (Local)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Jacksonville - Jaguars</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Indianapolis - Colts (Local)</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Miami - Dolphins (Local)</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>New York - Jets (Local)</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Tampa Bay - Buccaneers (Local)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Carolina - Panthers (Local)</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Seattle - Seahawks (Local)</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Buffalo - Bills</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Los Angeles - Chargers (Local)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Denver - Broncos</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>New England - Patriots (Local)</t>
+        </is>
+      </c>
+      <c r="R3" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Kenia Estefanía Cruz García</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Green Bay - Packers</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Dallas - Cowboys (Local)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Baltimore - Ravens (Local)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Philadelphia - Eagles (Local)</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>San Francisco - 49ers</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Jacksonville - Jaguars</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Houston - Texans</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Miami - Dolphins (Local)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Atlanta - Falcons</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Tampa Bay - Buccaneers (Local)</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Los Angeles - Rams</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Minnesota - Vikings</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Pittsburgh - Steelers (Local)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Los Angeles - Chargers (Local)</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Denver - Broncos</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>New England - Patriots (Local)</t>
+        </is>
+      </c>
+      <c r="R4" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Jaime Antonio García Morales</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Detroit - Lions (Local)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Dallas - Cowboys (Local)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Baltimore - Ravens (Local)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Philadelphia - Eagles (Local)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>San Francisco - 49ers</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Jacksonville - Jaguars</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Indianapolis - Colts (Local)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Miami - Dolphins (Local)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Atlanta - Falcons</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Tampa Bay - Buccaneers (Local)</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Los Angeles - Rams</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Seattle - Seahawks (Local)</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Buffalo - Bills</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Los Angeles - Chargers (Local)</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Denver - Broncos</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>New England - Patriots (Local)</t>
+        </is>
+      </c>
+      <c r="R5" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Arelí Olivas Alcántar</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Detroit - Lions (Local)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Kansas City - Chiefs</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Baltimore - Ravens (Local)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Philadelphia - Eagles (Local)</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>San Francisco - 49ers</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Jacksonville - Jaguars</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Indianapolis - Colts (Local)</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Miami - Dolphins (Local)</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Atlanta - Falcons</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Tampa Bay - Buccaneers (Local)</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Los Angeles - Rams</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Seattle - Seahawks (Local)</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Buffalo - Bills</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Los Angeles - Chargers (Local)</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Denver - Broncos</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>New England - Patriots (Local)</t>
+        </is>
+      </c>
+      <c r="R6" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Alberto Vargas Ortiz</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Detroit - Lions (Local)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Kansas City - Chiefs</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Baltimore - Ravens (Local)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Philadelphia - Eagles (Local)</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>San Francisco - 49ers</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Jacksonville - Jaguars</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Indianapolis - Colts (Local)</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Miami - Dolphins (Local)</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Atlanta - Falcons</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Tampa Bay - Buccaneers (Local)</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Los Angeles - Rams</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Seattle - Seahawks (Local)</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Buffalo - Bills</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Los Angeles - Chargers (Local)</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Denver - Broncos</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>New England - Patriots (Local)</t>
+        </is>
+      </c>
+      <c r="R7" t="n">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>